<commit_message>
added additional info to calculation spreadsheet
</commit_message>
<xml_diff>
--- a/ImageProcessing/Steganography/IndexMappingCalculations.xlsx
+++ b/ImageProcessing/Steganography/IndexMappingCalculations.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pietromalky/Desktop/Python Projects/ImageProcessing/Steganography/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19AD845B-A270-4B49-B814-DFD3A9299EF2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0259568E-EC52-3847-B02F-EB128B8C25DA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{53B7AC88-8130-B743-BECA-7C544673D638}"/>
   </bookViews>
   <sheets>
     <sheet name="FlatToRGB" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Flat Message Array</t>
   </si>
@@ -64,12 +64,21 @@
   </si>
   <si>
     <t>color bands</t>
+  </si>
+  <si>
+    <t>max hide size, MB</t>
+  </si>
+  <si>
+    <t>&lt;-- max file size that can be hidden given image's rows, cols and color channels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -152,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -166,12 +175,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -181,8 +184,20 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="1" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -501,7 +516,7 @@
   <dimension ref="B2:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -510,9 +525,9 @@
     <col min="2" max="2" width="17" style="1"/>
     <col min="3" max="3" width="5.83203125" style="1" customWidth="1"/>
     <col min="4" max="6" width="9" style="1" customWidth="1"/>
-    <col min="7" max="7" width="2.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="4.83203125" style="1" customWidth="1"/>
     <col min="8" max="9" width="17" style="1"/>
-    <col min="10" max="10" width="118.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="118.33203125" style="11" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="17" style="1"/>
   </cols>
   <sheetData>
@@ -520,37 +535,37 @@
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="H2" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="I2" s="6"/>
+      <c r="D2" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="H2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="9"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="9">
-        <v>200</v>
-      </c>
-      <c r="J3" s="10" t="s">
+      <c r="I3" s="7">
+        <v>1990</v>
+      </c>
+      <c r="J3" s="12" t="s">
         <v>3</v>
       </c>
     </row>
@@ -558,45 +573,45 @@
       <c r="B4" s="3">
         <v>0</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <f>_xlfn.FLOOR.MATH(B4/($I$5*$I$4))</f>
         <v>0</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <f>MOD(_xlfn.FLOOR.MATH(B4/$I$5),$I$4)</f>
         <v>0</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="6">
         <f>MOD(B4,$I$5)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="9">
-        <v>4</v>
+      <c r="I4" s="7">
+        <v>1580</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="3">
         <v>1</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <f t="shared" ref="D5:D36" si="0">_xlfn.FLOOR.MATH(B5/($I$5*$I$4))</f>
         <v>0</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="6">
         <f t="shared" ref="E5:E36" si="1">MOD(_xlfn.FLOOR.MATH(B5/$I$5),$I$4)</f>
         <v>0</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="6">
         <f t="shared" ref="F5:F36" si="2">MOD(B5,$I$5)</f>
         <v>1</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="H5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
         <v>3</v>
       </c>
     </row>
@@ -604,32 +619,42 @@
       <c r="B6" s="3">
         <v>2</v>
       </c>
-      <c r="D6" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="8">
-        <f t="shared" si="2"/>
-        <v>2</v>
+      <c r="D6" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" s="6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F6" s="6">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="10">
+        <f>I5 * I3 * I4 / (1024 * 1024)</f>
+        <v>8.9956283569335938</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="3">
         <v>3</v>
       </c>
-      <c r="D7" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F7" s="8">
+      <c r="D7" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -638,15 +663,15 @@
       <c r="B8" s="3">
         <v>4</v>
       </c>
-      <c r="D8" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E8" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F8" s="8">
+      <c r="D8" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F8" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -655,15 +680,15 @@
       <c r="B9" s="3">
         <v>5</v>
       </c>
-      <c r="D9" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F9" s="8">
+      <c r="D9" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -672,15 +697,15 @@
       <c r="B10" s="3">
         <v>6</v>
       </c>
-      <c r="D10" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F10" s="8">
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F10" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -689,15 +714,15 @@
       <c r="B11" s="3">
         <v>7</v>
       </c>
-      <c r="D11" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F11" s="8">
+      <c r="D11" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F11" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -706,15 +731,15 @@
       <c r="B12" s="3">
         <v>8</v>
       </c>
-      <c r="D12" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F12" s="8">
+      <c r="D12" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F12" s="6">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -723,15 +748,15 @@
       <c r="B13" s="3">
         <v>9</v>
       </c>
-      <c r="D13" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="8">
+      <c r="D13" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="6">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -740,15 +765,15 @@
       <c r="B14" s="3">
         <v>10</v>
       </c>
-      <c r="D14" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="8">
+      <c r="D14" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="6">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F14" s="8">
+      <c r="F14" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -757,15 +782,15 @@
       <c r="B15" s="3">
         <v>11</v>
       </c>
-      <c r="D15" s="8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="8">
+      <c r="D15" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="6">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="F15" s="8">
+      <c r="F15" s="6">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -774,15 +799,15 @@
       <c r="B16" s="3">
         <v>12</v>
       </c>
-      <c r="D16" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E16" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="8">
+      <c r="D16" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F16" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -791,15 +816,15 @@
       <c r="B17" s="3">
         <v>13</v>
       </c>
-      <c r="D17" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E17" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="8">
+      <c r="D17" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" s="6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F17" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -808,15 +833,15 @@
       <c r="B18" s="3">
         <v>14</v>
       </c>
-      <c r="D18" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E18" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="8">
+      <c r="D18" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" s="6">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F18" s="6">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -825,15 +850,15 @@
       <c r="B19" s="3">
         <v>15</v>
       </c>
-      <c r="D19" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E19" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F19" s="8">
+      <c r="D19" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F19" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -842,15 +867,15 @@
       <c r="B20" s="3">
         <v>16</v>
       </c>
-      <c r="D20" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E20" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F20" s="8">
+      <c r="D20" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" s="6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F20" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -859,15 +884,15 @@
       <c r="B21" s="3">
         <v>17</v>
       </c>
-      <c r="D21" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E21" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F21" s="8">
+      <c r="D21" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="F21" s="6">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -876,15 +901,15 @@
       <c r="B22" s="3">
         <v>18</v>
       </c>
-      <c r="D22" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E22" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F22" s="8">
+      <c r="D22" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" s="6">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F22" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -893,15 +918,15 @@
       <c r="B23" s="3">
         <v>19</v>
       </c>
-      <c r="D23" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E23" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F23" s="8">
+      <c r="D23" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E23" s="6">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F23" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -910,15 +935,15 @@
       <c r="B24" s="3">
         <v>20</v>
       </c>
-      <c r="D24" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E24" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F24" s="8">
+      <c r="D24" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24" s="6">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="F24" s="6">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -927,15 +952,15 @@
       <c r="B25" s="3">
         <v>21</v>
       </c>
-      <c r="D25" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E25" s="8">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F25" s="8">
+      <c r="D25" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" s="6">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F25" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -944,15 +969,15 @@
       <c r="B26" s="3">
         <v>22</v>
       </c>
-      <c r="D26" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E26" s="8">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F26" s="8">
+      <c r="D26" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26" s="6">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F26" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -961,15 +986,15 @@
       <c r="B27" s="3">
         <v>23</v>
       </c>
-      <c r="D27" s="8">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E27" s="8">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="F27" s="8">
+      <c r="D27" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="6">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="F27" s="6">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -978,15 +1003,15 @@
       <c r="B28" s="3">
         <v>24</v>
       </c>
-      <c r="D28" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E28" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F28" s="8">
+      <c r="D28" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E28" s="6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="F28" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -995,15 +1020,15 @@
       <c r="B29" s="3">
         <v>25</v>
       </c>
-      <c r="D29" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E29" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F29" s="8">
+      <c r="D29" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="F29" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1012,15 +1037,15 @@
       <c r="B30" s="3">
         <v>26</v>
       </c>
-      <c r="D30" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E30" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F30" s="8">
+      <c r="D30" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="F30" s="6">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -1029,15 +1054,15 @@
       <c r="B31" s="3">
         <v>27</v>
       </c>
-      <c r="D31" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E31" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F31" s="8">
+      <c r="D31" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" s="6">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F31" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1046,15 +1071,15 @@
       <c r="B32" s="3">
         <v>28</v>
       </c>
-      <c r="D32" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E32" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F32" s="8">
+      <c r="D32" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" s="6">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F32" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1063,15 +1088,15 @@
       <c r="B33" s="3">
         <v>29</v>
       </c>
-      <c r="D33" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E33" s="8">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="F33" s="8">
+      <c r="D33" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="6">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="F33" s="6">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
@@ -1080,15 +1105,15 @@
       <c r="B34" s="3">
         <v>30</v>
       </c>
-      <c r="D34" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E34" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F34" s="8">
+      <c r="D34" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E34" s="6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F34" s="6">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1097,15 +1122,15 @@
       <c r="B35" s="3">
         <v>31</v>
       </c>
-      <c r="D35" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E35" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F35" s="8">
+      <c r="D35" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F35" s="6">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
@@ -1114,15 +1139,15 @@
       <c r="B36" s="3">
         <v>32</v>
       </c>
-      <c r="D36" s="8">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E36" s="8">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="F36" s="8">
+      <c r="D36" s="6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="6">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="F36" s="6">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>

</xml_diff>